<commit_message>
Floating Interest Rates T1
</commit_message>
<xml_diff>
--- a/Mifos Automation Excels/Client/3130-MS-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-FLAT-Regular-CASH-Newcreateloan1.xlsx
+++ b/Mifos Automation Excels/Client/3130-MS-EI-DB-DL-REC-NON-RNI-CTPD-DL-MD-TR-2-ONTIME-OVERDUE-FEE-FLAT-Regular-CASH-Newcreateloan1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="NewLoanInput" sheetId="5" r:id="rId1"/>
@@ -638,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,8 +760,8 @@
         <v>42005</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>43</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -784,8 +784,8 @@
         <v>42005</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="14" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -1311,7 +1311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>

</xml_diff>